<commit_message>
version estable, todo ok. falta insertar producto
</commit_message>
<xml_diff>
--- a/PlanificacionProyecto4.xlsx
+++ b/PlanificacionProyecto4.xlsx
@@ -1,24 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\XAMP\DAW\Proyectos\PROYECTO4\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7665" tabRatio="630"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7668" tabRatio="630"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="3" r:id="rId2"/>
     <sheet name="Hoja4" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -26,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="77">
   <si>
     <t>Miercoles</t>
   </si>
@@ -254,13 +249,16 @@
   </si>
   <si>
     <t>Columna1</t>
+  </si>
+  <si>
+    <t>en desarrollo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -538,7 +536,7 @@
           <bgColor theme="0"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -555,7 +553,7 @@
           <bgColor theme="0"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -572,7 +570,7 @@
           <bgColor theme="0"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -589,7 +587,7 @@
           <bgColor theme="0"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -606,7 +604,7 @@
           <bgColor theme="0"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -623,13 +621,13 @@
           <bgColor theme="0"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -649,7 +647,7 @@
           <bgColor theme="0" tint="-0.14999847407452621"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -658,7 +656,7 @@
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -667,7 +665,7 @@
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -676,7 +674,7 @@
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -685,7 +683,7 @@
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -694,7 +692,7 @@
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -703,7 +701,7 @@
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -712,7 +710,7 @@
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -721,7 +719,7 @@
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -730,7 +728,7 @@
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -750,7 +748,7 @@
           <bgColor rgb="FF9AFAB1"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -839,7 +837,7 @@
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Tabla11" displayName="Tabla11" ref="D3:E15" totalsRowCount="1">
-  <autoFilter ref="D3:E15"/>
+  <autoFilter ref="D3:E14"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Fechas"/>
     <tableColumn id="2" name="Columna1" totalsRowFunction="custom">
@@ -893,7 +891,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -928,7 +926,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1105,33 +1103,33 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" customWidth="1"/>
     <col min="2" max="2" width="57" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" customWidth="1"/>
-    <col min="7" max="7" width="24.85546875" customWidth="1"/>
-    <col min="8" max="8" width="19.42578125" customWidth="1"/>
+    <col min="3" max="3" width="18.44140625" customWidth="1"/>
+    <col min="4" max="4" width="19.88671875" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" customWidth="1"/>
+    <col min="7" max="7" width="24.88671875" customWidth="1"/>
+    <col min="8" max="8" width="19.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="32.25" customHeight="1">
       <c r="A3" s="3" t="s">
         <v>13</v>
       </c>
@@ -1157,7 +1155,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="12" t="s">
         <v>14</v>
       </c>
@@ -1183,7 +1181,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="12" t="s">
         <v>15</v>
       </c>
@@ -1209,7 +1207,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="12" t="s">
         <v>16</v>
       </c>
@@ -1235,7 +1233,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="12" t="s">
         <v>17</v>
       </c>
@@ -1261,7 +1259,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" s="12" t="s">
         <v>18</v>
       </c>
@@ -1287,7 +1285,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" s="12" t="s">
         <v>19</v>
       </c>
@@ -1313,7 +1311,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" s="12" t="s">
         <v>20</v>
       </c>
@@ -1327,7 +1325,7 @@
         <v>1</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>47</v>
@@ -1339,7 +1337,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="12" t="s">
         <v>21</v>
       </c>
@@ -1365,7 +1363,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" s="12" t="s">
         <v>22</v>
       </c>
@@ -1391,7 +1389,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" s="12" t="s">
         <v>23</v>
       </c>
@@ -1417,7 +1415,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" s="12" t="s">
         <v>24</v>
       </c>
@@ -1443,7 +1441,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" s="12" t="s">
         <v>25</v>
       </c>
@@ -1469,7 +1467,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" s="12" t="s">
         <v>26</v>
       </c>
@@ -1495,7 +1493,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8">
       <c r="A17" s="12" t="s">
         <v>27</v>
       </c>
@@ -1521,7 +1519,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="A18" s="12" t="s">
         <v>28</v>
       </c>
@@ -1547,7 +1545,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="A19" s="12" t="s">
         <v>29</v>
       </c>
@@ -1573,7 +1571,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8">
       <c r="A20" s="12" t="s">
         <v>33</v>
       </c>
@@ -1587,7 +1585,7 @@
         <v>0</v>
       </c>
       <c r="E20" s="22" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="F20" s="29" t="s">
         <v>74</v>
@@ -1599,7 +1597,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8">
       <c r="A21" s="10" t="s">
         <v>34</v>
       </c>
@@ -1616,7 +1614,7 @@
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
     </row>
-    <row r="22" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" s="26" customFormat="1">
       <c r="A22" s="25" t="s">
         <v>34</v>
       </c>
@@ -1632,7 +1630,7 @@
       <c r="G22" s="24"/>
       <c r="H22" s="24"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8">
       <c r="A23" s="8" t="s">
         <v>34</v>
       </c>
@@ -1683,19 +1681,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A4:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="6" width="30.7109375" customWidth="1"/>
+    <col min="1" max="6" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="30" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -1715,7 +1713,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="30" customHeight="1">
       <c r="A5" s="20" t="s">
         <v>14</v>
       </c>
@@ -1735,7 +1733,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="30" customHeight="1">
       <c r="A6" s="20" t="s">
         <v>15</v>
       </c>
@@ -1753,7 +1751,7 @@
       </c>
       <c r="F6" s="20"/>
     </row>
-    <row r="7" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="30" customHeight="1">
       <c r="A7" s="20" t="s">
         <v>16</v>
       </c>
@@ -1771,7 +1769,7 @@
       </c>
       <c r="F7" s="20"/>
     </row>
-    <row r="8" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="30" customHeight="1">
       <c r="A8" s="1"/>
       <c r="B8" s="20" t="s">
         <v>20</v>
@@ -1785,7 +1783,7 @@
       </c>
       <c r="F8" s="20"/>
     </row>
-    <row r="9" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="30" customHeight="1">
       <c r="A9" s="1"/>
       <c r="B9" s="20" t="s">
         <v>21</v>
@@ -1795,7 +1793,7 @@
       <c r="E9" s="20"/>
       <c r="F9" s="20"/>
     </row>
-    <row r="10" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="30" customHeight="1">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1803,7 +1801,7 @@
       <c r="E10" s="20"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="30" customHeight="1">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1811,7 +1809,7 @@
       <c r="E11" s="20"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="30" customHeight="1">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1855,20 +1853,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" customWidth="1"/>
     <col min="3" max="4" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5">
       <c r="B3" t="s">
         <v>48</v>
       </c>
@@ -1882,7 +1880,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5">
       <c r="B4" t="s">
         <v>36</v>
       </c>
@@ -1896,7 +1894,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5">
       <c r="B5" t="s">
         <v>39</v>
       </c>
@@ -1910,7 +1908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5">
       <c r="B6" t="s">
         <v>40</v>
       </c>
@@ -1924,7 +1922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:5">
       <c r="D7" t="s">
         <v>47</v>
       </c>
@@ -1932,7 +1930,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:5">
       <c r="D8" t="s">
         <v>54</v>
       </c>
@@ -1940,7 +1938,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:5">
       <c r="D9" t="s">
         <v>37</v>
       </c>
@@ -1948,7 +1946,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:5">
       <c r="D10" t="s">
         <v>43</v>
       </c>
@@ -1956,7 +1954,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:5">
       <c r="D11" t="s">
         <v>55</v>
       </c>
@@ -1964,7 +1962,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:5">
       <c r="D12" t="s">
         <v>72</v>
       </c>
@@ -1972,7 +1970,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:5">
       <c r="D13" t="s">
         <v>73</v>
       </c>
@@ -1980,7 +1978,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:5">
       <c r="D14" t="s">
         <v>74</v>
       </c>
@@ -1988,7 +1986,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:5">
       <c r="E15">
         <f>SUM(E4:E14)</f>
         <v>42</v>

</xml_diff>